<commit_message>
Practica 2 casi acabada
</commit_message>
<xml_diff>
--- a/practica_02/datos.xlsx
+++ b/practica_02/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PLS\Universidad\10 - Cuatrimestre 5B\Teoría de Estructuras\03 - Laboratorio\Práctica 02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PLS\Universidad\10 - Cuatrimestre 5B\Teoría de Estructuras\03 - Laboratorio\practica_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F72840F-2FC3-475C-8B04-9EDB5AE8D062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F86DB6-1E88-474C-A38E-06DDEE00DD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0684A4E-88C8-4389-A260-F512C2FEEDC0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Carga [N]</t>
   </si>
@@ -76,13 +76,34 @@
     <t>Tensión [MPa]</t>
   </si>
   <si>
-    <t>Tensión Vs [mV]</t>
+    <t>Masa [kg]</t>
+  </si>
+  <si>
+    <t>Vs [mV]</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>ec</t>
+  </si>
+  <si>
+    <t>Rg [Ohm]</t>
+  </si>
+  <si>
+    <t>Rc [Ohm]</t>
+  </si>
+  <si>
+    <t>e [adim]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -130,6 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF64A176-AA00-4633-9835-D8679806315E}">
-  <dimension ref="B2:Q16"/>
+  <dimension ref="B2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,36 +480,61 @@
     <col min="8" max="17" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
         <v>0.245</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>29880</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5">
+        <f>F2/(F2+F3)*(1/F4)</f>
+        <v>1.9047619047619048E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -496,78 +543,41 @@
         <v>2.1333333333333332E-10</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="O9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11">
         <v>1819</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11">
-        <v>1807</v>
-      </c>
-      <c r="O11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P11">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="K13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1</v>
       </c>
@@ -575,33 +585,21 @@
         <f>9.81*B14</f>
         <v>9.81</v>
       </c>
-      <c r="F14">
+      <c r="D14">
         <v>280</v>
       </c>
-      <c r="G14" s="2">
+      <c r="E14" s="5">
+        <f>$F$5*D14/$C$11</f>
+        <v>2.9320139270661537E-4</v>
+      </c>
+      <c r="F14" s="2">
         <f>0.000001*6*$C$3*C14/($C$4*$C$5*$C$5)</f>
         <v>22.532343750000003</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>86</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
-        <f>9.81*O14</f>
-        <v>9.81</v>
-      </c>
-      <c r="Q14">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
@@ -609,33 +607,21 @@
         <f t="shared" ref="C15:C16" si="0">9.81*B15</f>
         <v>19.62</v>
       </c>
-      <c r="F15">
+      <c r="D15">
         <v>560</v>
       </c>
-      <c r="G15" s="2">
+      <c r="E15" s="5">
+        <f t="shared" ref="E15:E16" si="1">$F$5*D15/$C$11</f>
+        <v>5.8640278541323074E-4</v>
+      </c>
+      <c r="F15" s="2">
         <f>0.000001*6*$C$3*C15/($C$4*$C$5*$C$5)</f>
         <v>45.064687500000005</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="K15">
-        <v>2</v>
-      </c>
-      <c r="M15">
-        <v>174</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <f t="shared" ref="P15:P16" si="1">9.81*O15</f>
-        <v>19.62</v>
-      </c>
-      <c r="Q15">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>3</v>
       </c>
@@ -643,37 +629,125 @@
         <f t="shared" si="0"/>
         <v>29.43</v>
       </c>
-      <c r="F16">
+      <c r="D16">
         <v>840</v>
       </c>
-      <c r="G16" s="2">
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7960417811984611E-4</v>
+      </c>
+      <c r="F16" s="2">
         <f>0.000001*6*$C$3*C16/($C$4*$C$5*$C$5)</f>
         <v>67.597031250000001</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="K16">
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="F21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1807</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>86</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>9.81*F26</f>
+        <v>9.81</v>
+      </c>
+      <c r="H26">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>174</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ref="G27:G28" si="2">9.81*F27</f>
+        <v>19.62</v>
+      </c>
+      <c r="H27">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28">
         <v>3</v>
       </c>
-      <c r="M16">
+      <c r="D28">
         <v>260</v>
       </c>
-      <c r="O16">
+      <c r="F28">
         <v>3</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="1"/>
+      <c r="G28">
+        <f t="shared" si="2"/>
         <v>29.43</v>
       </c>
-      <c r="Q16">
+      <c r="H28">
         <v>1690</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="F21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>